<commit_message>
2017-07-02: add test case for model
</commit_message>
<xml_diff>
--- a/express/doc/POST参数/post参数.xlsx
+++ b/express/doc/POST参数/post参数.xlsx
@@ -382,11 +382,6 @@
     </r>
   </si>
   <si>
-    <t>一个字段对应fk字段的多个field，传递searchParams/filterFieldValue时，需要显式的指明fkField对应的记录中，对那个field进行查找/过滤
-例如，bill中，parentBillType定义为{coll:billType, allowFields:[field1,field2]}
-说明pararentBillType的值为objectId，可以通过对billType的field1或者field2进行查找，获得objectId数组，如果pararentBillType在此数组中存在，则取出。</t>
-  </si>
-  <si>
     <t>eventField</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -410,6 +405,12 @@
  to: eleArray中元素，要移动到哪个记录，如果没有，说明是删除
  eleArray:要操作的记录。可以为空数组
 }</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个字段对应fk字段的多个field，传递searchParams/filterFieldValue时，需要显式的指明fkField对应的记录中，对那个field进行查找/过滤
+例如，bill中，parentBillType定义为{coll:billType, allowFields:[field1,field2]}
+说明pararentBillType的值为objectId，可以通过对billType的field1或者field2进行查找，获得objectId数组，如果pararentBillType在此数组中存在，则取出。</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -799,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -836,10 +837,10 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="63.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -894,10 +895,10 @@
         <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.15">
@@ -989,7 +990,7 @@
     </row>
     <row r="9" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>

</xml_diff>

<commit_message>
2017-7-4: add 3 new coll and their related rule and test case
</commit_message>
<xml_diff>
--- a/express/doc/POST参数/post参数.xlsx
+++ b/express/doc/POST参数/post参数.xlsx
@@ -50,16 +50,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
-    <t>recorderInfo</t>
-  </si>
-  <si>
     <t>currentColl</t>
   </si>
   <si>
     <t>currentPage</t>
-  </si>
-  <si>
-    <t>recIdArr</t>
   </si>
   <si>
     <t>searchParams</t>
@@ -411,6 +405,14 @@
     <t>一个字段对应fk字段的多个field，传递searchParams/filterFieldValue时，需要显式的指明fkField对应的记录中，对那个field进行查找/过滤
 例如，bill中，parentBillType定义为{coll:billType, allowFields:[field1,field2]}
 说明pararentBillType的值为objectId，可以通过对billType的field1或者field2进行查找，获得objectId数组，如果pararentBillType在此数组中存在，则取出。</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>recordInfo</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>recIdArr</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -800,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -819,178 +821,178 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="63.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="41.25" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="127.5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>

</xml_diff>

<commit_message>
20170717: 1. add new part SINGLE_FIEL  2. user Ajax unique checke
</commit_message>
<xml_diff>
--- a/express/doc/POST参数/post参数.xlsx
+++ b/express/doc/POST参数/post参数.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ss_vue_express\express\doc\POST参数\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="28695" windowHeight="12990"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="28700" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +23,85 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>ZHANG Wei AG</author>
     <author>Ada</author>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ZHANG Wei AG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>对单个字段进行检查（例如检查用户唯一性已经密码的正确性
+采用现成的函数</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>validatePartFormat+validateCURecordInfoFormat</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>验证格式
+采用</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>validateSingleRecorderFieldValue</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>验证单个值</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
   <si>
     <t>currentColl</t>
   </si>
@@ -415,12 +495,20 @@
     <t>recIdArr</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>singleFieldValue</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>field:{value:xxx}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +544,26 @@
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -508,6 +616,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -800,26 +911,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.25" customWidth="1"/>
-    <col min="2" max="2" width="45.375" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="19.875" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="43.625" customWidth="1"/>
-    <col min="7" max="7" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="57.125" customWidth="1"/>
-    <col min="9" max="9" width="54.375" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="2" max="2" width="45.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="43.6328125" customWidth="1"/>
+    <col min="7" max="7" width="23.90625" customWidth="1"/>
+    <col min="8" max="8" width="57.08984375" customWidth="1"/>
+    <col min="9" max="9" width="54.36328125" customWidth="1"/>
+    <col min="10" max="10" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -844,8 +956,11 @@
       <c r="I1" t="s">
         <v>20</v>
       </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="63.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -873,8 +988,11 @@
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="112" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -902,8 +1020,11 @@
       <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="56.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -931,8 +1052,11 @@
       <c r="I4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J4" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="41.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -960,8 +1084,11 @@
       <c r="I5" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J5" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" ht="127.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="143" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -990,7 +1117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -1007,8 +1134,8 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1018,7 +1145,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1032,7 +1159,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2017-07-19: 1. add dispatcher to router CRUD to different bussiness logic code.   2. add new part METHOD
</commit_message>
<xml_diff>
--- a/express/doc/POST参数/post参数.xlsx
+++ b/express/doc/POST参数/post参数.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="60" windowWidth="28700" windowHeight="12990"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="part" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -123,12 +123,46 @@
         </r>
       </text>
     </comment>
+    <comment ref="K6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ZHANG Wei AG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>判断输入记录是否和db中存储的一直（例如登录）</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>currentColl</t>
   </si>
@@ -496,11 +530,19 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>singleFieldValue</t>
+    <t>field:{value:xxx}</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>field:{value:xxx}</t>
+    <t>method</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>singleField</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>match:4</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -508,7 +550,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,6 +607,14 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -588,7 +638,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -605,6 +655,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -911,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -931,7 +984,7 @@
     <col min="10" max="10" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -956,11 +1009,14 @@
       <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
-        <v>27</v>
+      <c r="J1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="64" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -989,10 +1045,13 @@
         <v>8</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="112" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="112" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1021,10 +1080,13 @@
         <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="56.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="56.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1053,10 +1115,13 @@
         <v>8</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1085,10 +1150,13 @@
         <v>8</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="143" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="143" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1116,8 +1184,11 @@
       <c r="I6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="K6" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>

</xml_diff>